<commit_message>
Simple basic untested client
</commit_message>
<xml_diff>
--- a/Api.xlsx
+++ b/Api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mt_xi\Documents\Projects\Websites\socketio-multiplayer-game-library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE9B637-F6E1-4B25-A608-980509C30FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048CC5B4-D323-4928-A56B-1D6E58DA6345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>